<commit_message>
Third Issue Basic Validation statistics
</commit_message>
<xml_diff>
--- a/data/STREAMLINING PROCESSES AT KINYANJUI FARM.xlsx
+++ b/data/STREAMLINING PROCESSES AT KINYANJUI FARM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\github-classroom\20230821-20231128-BI2-BBIT4-2\BIAcersProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29466CEC-DA92-407F-A029-1E769A24CB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B51DBA-7F22-4E88-8E93-A87F78484632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,24 +30,12 @@
     <t>NAMES</t>
   </si>
   <si>
-    <t xml:space="preserve">TOTAL KGS </t>
-  </si>
-  <si>
     <t>AMOUNT</t>
   </si>
   <si>
-    <t xml:space="preserve">TOTAL DAYS </t>
-  </si>
-  <si>
-    <t>TOTAL AMOUNT</t>
-  </si>
-  <si>
     <t>ADVANCE</t>
   </si>
   <si>
-    <t>NET PAY</t>
-  </si>
-  <si>
     <t>Jane Therero</t>
   </si>
   <si>
@@ -142,6 +130,18 @@
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTALKGS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTALDAYS </t>
+  </si>
+  <si>
+    <t>TOTALAMOUNT</t>
+  </si>
+  <si>
+    <t>NETPAY</t>
   </si>
 </sst>
 </file>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,33 +482,33 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>1454</v>
@@ -529,12 +529,12 @@
         <v>12530</v>
       </c>
       <c r="I2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>607</v>
@@ -558,12 +558,12 @@
         <v>4555</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>349</v>
@@ -581,12 +581,12 @@
         <v>1290</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>244</v>
@@ -610,12 +610,12 @@
         <v>1550</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>502</v>
@@ -639,12 +639,12 @@
         <v>3315</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>710</v>
@@ -668,12 +668,12 @@
         <v>5785</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>385</v>
@@ -691,12 +691,12 @@
         <v>2165</v>
       </c>
       <c r="I8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>537</v>
@@ -714,12 +714,12 @@
         <v>3245</v>
       </c>
       <c r="I9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>632</v>
@@ -737,12 +737,12 @@
         <v>3755</v>
       </c>
       <c r="I10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>379</v>
@@ -766,12 +766,12 @@
         <v>2330</v>
       </c>
       <c r="I11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>270</v>
@@ -789,12 +789,12 @@
         <v>100</v>
       </c>
       <c r="I12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>960</v>
@@ -815,12 +815,12 @@
         <v>7980</v>
       </c>
       <c r="I13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>327</v>
@@ -838,12 +838,12 @@
         <v>2365</v>
       </c>
       <c r="I14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>356</v>
@@ -861,12 +861,12 @@
         <v>2050</v>
       </c>
       <c r="I15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>176</v>
@@ -884,12 +884,12 @@
         <v>410</v>
       </c>
       <c r="I16" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>534</v>
@@ -904,12 +904,12 @@
         <v>4270</v>
       </c>
       <c r="I17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>577</v>
@@ -933,12 +933,12 @@
         <v>4315</v>
       </c>
       <c r="I18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>471</v>
@@ -962,12 +962,12 @@
         <v>2820</v>
       </c>
       <c r="I19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>236</v>
@@ -985,12 +985,12 @@
         <v>240</v>
       </c>
       <c r="I20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>893</v>
@@ -1014,12 +1014,12 @@
         <v>5595</v>
       </c>
       <c r="I21" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>325</v>
@@ -1037,12 +1037,12 @@
         <v>1100</v>
       </c>
       <c r="I22" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>350</v>
@@ -1066,12 +1066,12 @@
         <v>2600</v>
       </c>
       <c r="I23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>183</v>
@@ -1095,12 +1095,12 @@
         <v>1565</v>
       </c>
       <c r="I24" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>152</v>
@@ -1118,12 +1118,12 @@
         <v>1015</v>
       </c>
       <c r="I25" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B26">
         <v>403</v>
@@ -1141,12 +1141,12 @@
         <v>2925</v>
       </c>
       <c r="I26" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>18</v>
@@ -1158,12 +1158,12 @@
         <v>145</v>
       </c>
       <c r="I27" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B28">
         <v>88</v>
@@ -1181,12 +1181,12 @@
         <v>405</v>
       </c>
       <c r="I28" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B29">
         <v>62</v>
@@ -1207,12 +1207,12 @@
         <v>1095</v>
       </c>
       <c r="I29" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B30">
         <v>434</v>
@@ -1230,7 +1230,7 @@
         <v>2970</v>
       </c>
       <c r="I30" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>